<commit_message>
fix value type promotion bug
</commit_message>
<xml_diff>
--- a/test/data/othercase.xlsx
+++ b/test/data/othercase.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maste\.julia\dev\XLSXasJSON\test\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devsisters\.julia\dev\XLSXasJSON\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D23196B-999E-4988-8DFD-9BC16A6C1A50}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11835" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Missing" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="promotion" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>SMITH</t>
   </si>
@@ -76,13 +76,41 @@
   </si>
   <si>
     <t>It can be done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t1.A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t1.B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t2.A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t2.B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t3.A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t3.B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t3.C</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -434,10 +462,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -517,7 +545,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40DFBF20-ADF8-4C70-8AA9-B3287647E6E2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -540,4 +568,66 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0.5</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix merge bug and added test for merge
</commit_message>
<xml_diff>
--- a/test/data/othercase.xlsx
+++ b/test/data/othercase.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11835" activeTab="2"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11835" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Missing" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
     <sheet name="promotion" sheetId="4" r:id="rId3"/>
+    <sheet name="mergeA" sheetId="5" r:id="rId4"/>
+    <sheet name="mergeB" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>SMITH</t>
   </si>
@@ -104,6 +106,130 @@
   </si>
   <si>
     <t>t3.C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Some</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Place</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Beyond</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rainbow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>My</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Is</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jonas</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>York</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Los</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Angeles</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Property.[1,A]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Property.[2,A]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Out</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>of</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>idea</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cannot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>think</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>of</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>anything</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>funny</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Address.State</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Address.City</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>555;1111;2222</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>555;3333;4444</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>555;5555;6666</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>555;7777;8888</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Address.TEL(Int)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -574,7 +700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -630,4 +756,179 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
DELIM bug 임시 수정
</commit_message>
<xml_diff>
--- a/test/data/othercase.xlsx
+++ b/test/data/othercase.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11835" activeTab="3"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11835" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Missing" sheetId="2" r:id="rId1"/>
@@ -17,8 +17,9 @@
     <sheet name="promotion" sheetId="4" r:id="rId3"/>
     <sheet name="mergeA" sheetId="5" r:id="rId4"/>
     <sheet name="mergeB" sheetId="6" r:id="rId5"/>
+    <sheet name="adddelim" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
   <si>
     <t>SMITH</t>
   </si>
@@ -230,6 +231,34 @@
   </si>
   <si>
     <t>Address.TEL(Int)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Array_1()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a,b,c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d,e,f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Array_2(Int)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4,5,6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -701,7 +730,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G2" sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -762,8 +791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -931,4 +960,53 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
move delim to keward argument for worksheet
</commit_message>
<xml_diff>
--- a/test/data/othercase.xlsx
+++ b/test/data/othercase.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devsisters\.julia\dev\XLSXasJSON\test\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Masterplan\.julia\dev\XLSXasJSON\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED70E9FC-BB4F-45EA-91B7-59A60A9C43A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11835" activeTab="5"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Missing" sheetId="2" r:id="rId1"/>
@@ -17,7 +18,6 @@
     <sheet name="promotion" sheetId="4" r:id="rId3"/>
     <sheet name="mergeA" sheetId="5" r:id="rId4"/>
     <sheet name="mergeB" sheetId="6" r:id="rId5"/>
-    <sheet name="adddelim" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>SMITH</t>
   </si>
@@ -231,41 +231,13 @@
   </si>
   <si>
     <t>Address.TEL(Int)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Index</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Array_1()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>a,b,c</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>d,e,f</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Array_2(Int)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1,2,3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4,5,6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -617,16 +589,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.5" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -640,7 +612,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -651,7 +623,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -665,7 +637,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -673,7 +645,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -681,7 +653,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -700,21 +672,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -726,16 +698,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -758,7 +730,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -788,19 +760,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="9.88671875" customWidth="1"/>
+    <col min="2" max="2" width="9.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -814,7 +786,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -828,7 +800,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -842,7 +814,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -856,7 +828,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -877,16 +849,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -900,7 +872,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -914,7 +886,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -928,7 +900,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -942,7 +914,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -954,55 +926,6 @@
       </c>
       <c r="D5" t="s">
         <v>46</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>